<commit_message>
feat: Implementar gestión de archivos recientes y mejorar UI
- Agregar ConfigManager para persistencia de configuración
- Implementar Combobox para selección de archivos recientes
- Recordar última hoja usada por archivo
- Unificar selección de propiedad con opción 'Sin Logo'
- Mejorar diseño y espaciado de la interfaz
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3995" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3998" uniqueCount="731">
   <si>
     <t xml:space="preserve">HAB</t>
   </si>
@@ -1924,6 +1924,9 @@
     <t xml:space="preserve">encryption</t>
   </si>
   <si>
+    <t xml:space="preserve">propiedad</t>
+  </si>
+  <si>
     <t xml:space="preserve">1301</t>
   </si>
   <si>
@@ -1945,6 +1948,9 @@
     <t xml:space="preserve">WPA2</t>
   </si>
   <si>
+    <t xml:space="preserve">vle</t>
+  </si>
+  <si>
     <t xml:space="preserve">habitación vacía</t>
   </si>
   <si>
@@ -1958,6 +1964,9 @@
   </si>
   <si>
     <t xml:space="preserve">WPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vg</t>
   </si>
   <si>
     <t xml:space="preserve">192.168.200.64/27</t>
@@ -5114,9 +5123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>630720</xdr:colOff>
+      <xdr:colOff>630360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5125,13 +5134,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="19410" t="33612" r="45501" b="25020"/>
+        <a:srcRect l="19407" t="33607" r="45496" b="25015"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2358000" y="12960"/>
-          <a:ext cx="3174840" cy="1947960"/>
+          <a:ext cx="3174480" cy="1947600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5158,9 +5167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>630720</xdr:colOff>
+      <xdr:colOff>630360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5169,13 +5178,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="19410" t="33612" r="45501" b="25020"/>
+        <a:srcRect l="19407" t="33607" r="45496" b="25015"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2358000" y="12960"/>
-          <a:ext cx="3174840" cy="1947960"/>
+          <a:ext cx="3174480" cy="1947600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10690,10 +10699,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1052"/>
+  <dimension ref="A1:Q1052"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10768,10 +10777,13 @@
       <c r="P1" s="220" t="s">
         <v>576</v>
       </c>
+      <c r="Q1" s="220" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="381" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B2" s="386" t="str">
         <f aca="false">LEFT(A2)</f>
@@ -10787,19 +10799,19 @@
         <v>45773</v>
       </c>
       <c r="F2" s="220" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G2" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H2" s="220" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="I2" s="220" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="J2" s="220" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="K2" s="220" t="n">
         <v>1001</v>
@@ -10813,7 +10825,10 @@
         <v>LaEstancia1301</v>
       </c>
       <c r="P2" s="220" t="s">
-        <v>583</v>
+        <v>584</v>
+      </c>
+      <c r="Q2" s="220" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10831,19 +10846,19 @@
         <v>418</v>
       </c>
       <c r="E3" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G3" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H3" s="220" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="I3" s="220" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="J3" s="220" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="K3" s="220" t="n">
         <v>1002</v>
@@ -10857,7 +10872,10 @@
         <v>LaEstancia1103A</v>
       </c>
       <c r="P3" s="220" t="s">
-        <v>588</v>
+        <v>590</v>
+      </c>
+      <c r="Q3" s="220" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10878,16 +10896,16 @@
         <v>45772</v>
       </c>
       <c r="G4" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H4" s="220" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="I4" s="220" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="J4" s="220" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="K4" s="220" t="n">
         <v>1003</v>
@@ -10901,12 +10919,12 @@
         <v>LaEstancia1103B</v>
       </c>
       <c r="P4" s="220" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="381" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B5" s="220" t="str">
         <f aca="false">LEFT(A5)</f>
@@ -10922,16 +10940,16 @@
         <v>45773</v>
       </c>
       <c r="F5" s="220" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G5" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H5" s="220" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="I5" s="220" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="J5" s="387" t="n">
         <v>192168200127</v>
@@ -10967,13 +10985,13 @@
         <v>45773</v>
       </c>
       <c r="G6" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H6" s="220" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="I6" s="220" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="J6" s="387" t="n">
         <v>192168200159</v>
@@ -11009,13 +11027,13 @@
         <v>45773</v>
       </c>
       <c r="G7" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H7" s="220" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="I7" s="220" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="J7" s="387" t="n">
         <v>192168200191</v>
@@ -11051,13 +11069,13 @@
         <v>45772</v>
       </c>
       <c r="G8" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H8" s="220" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="I8" s="220" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="J8" s="387" t="n">
         <v>192168200223</v>
@@ -11093,13 +11111,13 @@
         <v>45771</v>
       </c>
       <c r="G9" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H9" s="220" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="I9" s="220" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="J9" s="387" t="n">
         <v>192168200255</v>
@@ -11125,7 +11143,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="220" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D10" s="381" t="str">
         <f aca="false" t="array" ref="D10:D10">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11135,16 +11153,16 @@
         <v>45774</v>
       </c>
       <c r="G10" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H10" s="220" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="I10" s="220" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="J10" s="220" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="K10" s="220" t="n">
         <v>1009</v>
@@ -11177,16 +11195,16 @@
         <v>45771</v>
       </c>
       <c r="G11" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H11" s="220" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="I11" s="220" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="J11" s="220" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="K11" s="220" t="n">
         <v>1010</v>
@@ -11209,7 +11227,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="388" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D12" s="389" t="str">
         <f aca="false" t="array" ref="D12:D12">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11219,16 +11237,16 @@
         <v>45770</v>
       </c>
       <c r="G12" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H12" s="220" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="I12" s="220" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="J12" s="220" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="K12" s="220" t="n">
         <v>1011</v>
@@ -11258,16 +11276,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E13" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G13" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H13" s="220" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="I13" s="220" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="J13" s="387" t="n">
         <v>192168201127</v>
@@ -11303,13 +11321,13 @@
         <v>45771</v>
       </c>
       <c r="G14" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H14" s="220" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="I14" s="220" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J14" s="387" t="n">
         <v>192168201159</v>
@@ -11345,13 +11363,13 @@
         <v>45776</v>
       </c>
       <c r="G15" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H15" s="220" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="I15" s="220" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="J15" s="387" t="n">
         <v>192168201191</v>
@@ -11387,13 +11405,13 @@
         <v>45774</v>
       </c>
       <c r="G16" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H16" s="220" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="I16" s="220" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="J16" s="387" t="n">
         <v>192168201223</v>
@@ -11429,13 +11447,13 @@
         <v>45779</v>
       </c>
       <c r="G17" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H17" s="220" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="I17" s="220" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="J17" s="387" t="n">
         <v>192168201255</v>
@@ -11471,16 +11489,16 @@
         <v>45779</v>
       </c>
       <c r="G18" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H18" s="220" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="I18" s="220" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="J18" s="220" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="K18" s="220" t="n">
         <v>1017</v>
@@ -11513,16 +11531,16 @@
         <v>45770</v>
       </c>
       <c r="G19" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H19" s="220" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="I19" s="220" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="J19" s="220" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="K19" s="220" t="n">
         <v>1018</v>
@@ -11552,19 +11570,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E20" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G20" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H20" s="220" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="I20" s="220" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="J20" s="220" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="K20" s="220" t="n">
         <v>1019</v>
@@ -11587,7 +11605,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="220" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D21" s="220" t="str">
         <f aca="false" t="array" ref="D21:D21">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11597,13 +11615,13 @@
         <v>45770</v>
       </c>
       <c r="G21" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H21" s="220" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="I21" s="220" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="J21" s="387" t="n">
         <v>192168202127</v>
@@ -11629,7 +11647,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="388" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="D22" s="388" t="str">
         <f aca="false" t="array" ref="D22:D22">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11639,13 +11657,13 @@
         <v>45770</v>
       </c>
       <c r="G22" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H22" s="220" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="I22" s="220" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="J22" s="387" t="n">
         <v>192168202159</v>
@@ -11681,13 +11699,13 @@
         <v>45773</v>
       </c>
       <c r="G23" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H23" s="220" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="I23" s="220" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="J23" s="387" t="n">
         <v>192168202191</v>
@@ -11713,7 +11731,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="220" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D24" s="220" t="str">
         <f aca="false" t="array" ref="D24:D24">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11723,13 +11741,13 @@
         <v>45771</v>
       </c>
       <c r="G24" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H24" s="220" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="I24" s="220" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="J24" s="387" t="n">
         <v>192168202223</v>
@@ -11762,16 +11780,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E25" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G25" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H25" s="220" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="I25" s="220" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="J25" s="387" t="n">
         <v>192168202255</v>
@@ -11804,19 +11822,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E26" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G26" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H26" s="220" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="I26" s="220" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="J26" s="220" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="K26" s="220" t="n">
         <v>1025</v>
@@ -11846,19 +11864,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E27" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G27" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H27" s="220" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="I27" s="220" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="J27" s="220" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="K27" s="220" t="n">
         <v>1026</v>
@@ -11881,7 +11899,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="220" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D28" s="220" t="str">
         <f aca="false" t="array" ref="D28:D28">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11891,16 +11909,16 @@
         <v>45774</v>
       </c>
       <c r="G28" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H28" s="220" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="I28" s="220" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="J28" s="220" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="K28" s="220" t="n">
         <v>1027</v>
@@ -11923,7 +11941,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="220" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D29" s="220" t="str">
         <f aca="false" t="array" ref="D29:D29">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -11933,13 +11951,13 @@
         <v>45770</v>
       </c>
       <c r="G29" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H29" s="220" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="I29" s="220" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="J29" s="387" t="n">
         <v>192168203127</v>
@@ -11975,13 +11993,13 @@
         <v>45775</v>
       </c>
       <c r="G30" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H30" s="220" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="I30" s="220" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="J30" s="387" t="n">
         <v>192168203159</v>
@@ -12007,7 +12025,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="220" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D31" s="220" t="str">
         <f aca="false" t="array" ref="D31:D31">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12017,13 +12035,13 @@
         <v>45775</v>
       </c>
       <c r="G31" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H31" s="220" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="I31" s="220" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="J31" s="387" t="n">
         <v>192168203191</v>
@@ -12049,7 +12067,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="220" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D32" s="220" t="str">
         <f aca="false" t="array" ref="D32:D32">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12059,13 +12077,13 @@
         <v>45778</v>
       </c>
       <c r="G32" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H32" s="220" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="I32" s="220" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="J32" s="387" t="n">
         <v>192168203223</v>
@@ -12101,13 +12119,13 @@
         <v>45778</v>
       </c>
       <c r="G33" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H33" s="220" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="I33" s="220" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="J33" s="387" t="n">
         <v>192168203255</v>
@@ -12133,26 +12151,26 @@
         <v>3</v>
       </c>
       <c r="C34" s="388" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D34" s="388" t="str">
         <f aca="false" t="array" ref="D34:D34">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E34" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G34" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H34" s="220" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I34" s="220" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="J34" s="220" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="K34" s="220" t="n">
         <v>1033</v>
@@ -12175,7 +12193,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="220" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="D35" s="220" t="str">
         <f aca="false" t="array" ref="D35:D35">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12185,16 +12203,16 @@
         <v>45770</v>
       </c>
       <c r="G35" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H35" s="220" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="I35" s="220" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="J35" s="220" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="K35" s="220" t="n">
         <v>1034</v>
@@ -12217,26 +12235,26 @@
         <v>3</v>
       </c>
       <c r="C36" s="220" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="D36" s="220" t="str">
         <f aca="false" t="array" ref="D36:D36">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E36" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G36" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H36" s="220" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="I36" s="220" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="J36" s="220" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="K36" s="220" t="n">
         <v>1035</v>
@@ -12259,7 +12277,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="220" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="D37" s="220" t="str">
         <f aca="false" t="array" ref="D37:D37">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12269,13 +12287,13 @@
         <v>45771</v>
       </c>
       <c r="G37" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H37" s="220" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="I37" s="220" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="J37" s="387" t="n">
         <v>192168204127</v>
@@ -12301,7 +12319,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="220" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D38" s="220" t="str">
         <f aca="false" t="array" ref="D38:D38">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12311,13 +12329,13 @@
         <v>45771</v>
       </c>
       <c r="G38" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H38" s="220" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="I38" s="220" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="J38" s="387" t="n">
         <v>192168204159</v>
@@ -12343,7 +12361,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="220" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D39" s="220" t="str">
         <f aca="false" t="array" ref="D39:D39">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -12353,13 +12371,13 @@
         <v>45774</v>
       </c>
       <c r="G39" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H39" s="220" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="I39" s="220" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="J39" s="387" t="n">
         <v>192168204191</v>
@@ -12395,13 +12413,13 @@
         <v>45771</v>
       </c>
       <c r="G40" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H40" s="220" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="I40" s="220" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="J40" s="387" t="n">
         <v>192168204223</v>
@@ -12434,16 +12452,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E41" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G41" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H41" s="220" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="I41" s="220" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="J41" s="387" t="n">
         <v>192168204255</v>
@@ -12476,19 +12494,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E42" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G42" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H42" s="220" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="I42" s="220" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="J42" s="220" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="K42" s="220" t="n">
         <v>1041</v>
@@ -12521,16 +12539,16 @@
         <v>45771</v>
       </c>
       <c r="G43" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H43" s="220" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="I43" s="220" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="J43" s="220" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="K43" s="220" t="n">
         <v>1042</v>
@@ -12563,16 +12581,16 @@
         <v>45771</v>
       </c>
       <c r="G44" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H44" s="220" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="I44" s="220" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="J44" s="220" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="K44" s="220" t="n">
         <v>1043</v>
@@ -12605,13 +12623,13 @@
         <v>45771</v>
       </c>
       <c r="G45" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H45" s="220" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="I45" s="220" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="J45" s="387" t="n">
         <v>192168205127</v>
@@ -12647,13 +12665,13 @@
         <v>45772</v>
       </c>
       <c r="G46" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H46" s="220" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="I46" s="220" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="J46" s="387" t="n">
         <v>192168205159</v>
@@ -12689,13 +12707,13 @@
         <v>45774</v>
       </c>
       <c r="G47" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H47" s="220" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="I47" s="220" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="J47" s="387" t="n">
         <v>192168205191</v>
@@ -12731,13 +12749,13 @@
         <v>45774</v>
       </c>
       <c r="G48" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H48" s="220" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="I48" s="220" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="J48" s="387" t="n">
         <v>192168205223</v>
@@ -12773,13 +12791,13 @@
         <v>45773</v>
       </c>
       <c r="G49" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H49" s="220" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="I49" s="220" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="J49" s="387" t="n">
         <v>192168205255</v>
@@ -12815,16 +12833,16 @@
         <v>45772</v>
       </c>
       <c r="G50" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H50" s="220" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="I50" s="220" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="J50" s="220" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="K50" s="220" t="n">
         <v>1049</v>
@@ -12854,19 +12872,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E51" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G51" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H51" s="220" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="I51" s="220" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="J51" s="220" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="K51" s="220" t="n">
         <v>1050</v>
@@ -12882,7 +12900,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="381" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B52" s="220" t="str">
         <f aca="false">LEFT(A52)</f>
@@ -12896,13 +12914,13 @@
       <c r="F52" s="382"/>
       <c r="G52" s="221"/>
       <c r="H52" s="220" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="I52" s="220" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="J52" s="220" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="K52" s="220" t="n">
         <v>1051</v>
@@ -12911,7 +12929,7 @@
         <v>123456789</v>
       </c>
       <c r="O52" s="220" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16030,7 +16048,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="220" width="17.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="16" style="220" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="220" width="46.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="81" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16082,7 +16100,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="381" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B2" s="386" t="str">
         <f aca="false">LEFT(A2)</f>
@@ -16098,19 +16116,19 @@
         <v>45773</v>
       </c>
       <c r="F2" s="220" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G2" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H2" s="220" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="I2" s="220" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="J2" s="220" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="K2" s="220" t="n">
         <v>1001</v>
@@ -16139,19 +16157,19 @@
         <v>418</v>
       </c>
       <c r="E3" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G3" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H3" s="220" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="I3" s="220" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="J3" s="220" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="K3" s="220" t="n">
         <v>1002</v>
@@ -16183,16 +16201,16 @@
         <v>45772</v>
       </c>
       <c r="G4" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H4" s="220" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="I4" s="220" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="J4" s="220" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="K4" s="220" t="n">
         <v>1003</v>
@@ -16208,7 +16226,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="381" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B5" s="220" t="str">
         <f aca="false">LEFT(A5)</f>
@@ -16224,16 +16242,16 @@
         <v>45773</v>
       </c>
       <c r="F5" s="220" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G5" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H5" s="220" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="I5" s="220" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="J5" s="387" t="n">
         <v>192168200127</v>
@@ -16269,13 +16287,13 @@
         <v>45773</v>
       </c>
       <c r="G6" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H6" s="220" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="I6" s="220" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="J6" s="387" t="n">
         <v>192168200159</v>
@@ -16311,13 +16329,13 @@
         <v>45773</v>
       </c>
       <c r="G7" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H7" s="220" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="I7" s="220" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="J7" s="387" t="n">
         <v>192168200191</v>
@@ -16353,13 +16371,13 @@
         <v>45772</v>
       </c>
       <c r="G8" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H8" s="220" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="I8" s="220" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="J8" s="387" t="n">
         <v>192168200223</v>
@@ -16395,13 +16413,13 @@
         <v>45771</v>
       </c>
       <c r="G9" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H9" s="220" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="I9" s="220" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="J9" s="387" t="n">
         <v>192168200255</v>
@@ -16427,7 +16445,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="220" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D10" s="381" t="str">
         <f aca="false" t="array" ref="D10:D10">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -16437,16 +16455,16 @@
         <v>45774</v>
       </c>
       <c r="G10" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H10" s="220" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="I10" s="220" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="J10" s="220" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="K10" s="220" t="n">
         <v>1009</v>
@@ -16479,16 +16497,16 @@
         <v>45771</v>
       </c>
       <c r="G11" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H11" s="220" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="I11" s="220" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="J11" s="220" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="K11" s="220" t="n">
         <v>1010</v>
@@ -16511,7 +16529,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="388" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D12" s="389" t="str">
         <f aca="false" t="array" ref="D12:D12">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -16521,16 +16539,16 @@
         <v>45770</v>
       </c>
       <c r="G12" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H12" s="220" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="I12" s="220" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="J12" s="220" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="K12" s="220" t="n">
         <v>1011</v>
@@ -16560,16 +16578,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E13" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G13" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H13" s="220" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="I13" s="220" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="J13" s="387" t="n">
         <v>192168201127</v>
@@ -16605,13 +16623,13 @@
         <v>45771</v>
       </c>
       <c r="G14" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H14" s="220" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="I14" s="220" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="J14" s="387" t="n">
         <v>192168201159</v>
@@ -16647,13 +16665,13 @@
         <v>45776</v>
       </c>
       <c r="G15" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H15" s="220" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="I15" s="220" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="J15" s="387" t="n">
         <v>192168201191</v>
@@ -16689,13 +16707,13 @@
         <v>45774</v>
       </c>
       <c r="G16" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H16" s="220" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="I16" s="220" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="J16" s="387" t="n">
         <v>192168201223</v>
@@ -16731,13 +16749,13 @@
         <v>45779</v>
       </c>
       <c r="G17" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H17" s="220" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="I17" s="220" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="J17" s="387" t="n">
         <v>192168201255</v>
@@ -16773,16 +16791,16 @@
         <v>45779</v>
       </c>
       <c r="G18" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H18" s="220" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="I18" s="220" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="J18" s="220" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="K18" s="220" t="n">
         <v>1017</v>
@@ -16815,16 +16833,16 @@
         <v>45770</v>
       </c>
       <c r="G19" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H19" s="220" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="I19" s="220" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="J19" s="220" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="K19" s="220" t="n">
         <v>1018</v>
@@ -16854,19 +16872,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E20" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G20" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H20" s="220" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="I20" s="220" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="J20" s="220" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="K20" s="220" t="n">
         <v>1019</v>
@@ -16889,7 +16907,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="220" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D21" s="220" t="str">
         <f aca="false" t="array" ref="D21:D21">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -16899,13 +16917,13 @@
         <v>45770</v>
       </c>
       <c r="G21" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H21" s="220" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="I21" s="220" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="J21" s="387" t="n">
         <v>192168202127</v>
@@ -16931,7 +16949,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="388" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="D22" s="388" t="str">
         <f aca="false" t="array" ref="D22:D22">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -16941,13 +16959,13 @@
         <v>45770</v>
       </c>
       <c r="G22" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H22" s="220" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="I22" s="220" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="J22" s="387" t="n">
         <v>192168202159</v>
@@ -16983,13 +17001,13 @@
         <v>45773</v>
       </c>
       <c r="G23" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H23" s="220" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="I23" s="220" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="J23" s="387" t="n">
         <v>192168202191</v>
@@ -17015,7 +17033,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="220" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D24" s="220" t="str">
         <f aca="false" t="array" ref="D24:D24">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17025,13 +17043,13 @@
         <v>45771</v>
       </c>
       <c r="G24" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H24" s="220" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="I24" s="220" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="J24" s="387" t="n">
         <v>192168202223</v>
@@ -17064,16 +17082,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E25" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G25" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H25" s="220" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="I25" s="220" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="J25" s="387" t="n">
         <v>192168202255</v>
@@ -17106,19 +17124,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E26" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G26" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H26" s="220" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="I26" s="220" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="J26" s="220" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="K26" s="220" t="n">
         <v>1025</v>
@@ -17148,19 +17166,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E27" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G27" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H27" s="220" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="I27" s="220" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="J27" s="220" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="K27" s="220" t="n">
         <v>1026</v>
@@ -17183,7 +17201,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="220" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D28" s="220" t="str">
         <f aca="false" t="array" ref="D28:D28">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17193,16 +17211,16 @@
         <v>45774</v>
       </c>
       <c r="G28" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H28" s="220" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="I28" s="220" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="J28" s="220" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="K28" s="220" t="n">
         <v>1027</v>
@@ -17225,7 +17243,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="220" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D29" s="220" t="str">
         <f aca="false" t="array" ref="D29:D29">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17235,13 +17253,13 @@
         <v>45770</v>
       </c>
       <c r="G29" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H29" s="220" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="I29" s="220" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="J29" s="387" t="n">
         <v>192168203127</v>
@@ -17277,13 +17295,13 @@
         <v>45775</v>
       </c>
       <c r="G30" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H30" s="220" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="I30" s="220" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="J30" s="387" t="n">
         <v>192168203159</v>
@@ -17309,7 +17327,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="220" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D31" s="220" t="str">
         <f aca="false" t="array" ref="D31:D31">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17319,13 +17337,13 @@
         <v>45775</v>
       </c>
       <c r="G31" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H31" s="220" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="I31" s="220" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="J31" s="387" t="n">
         <v>192168203191</v>
@@ -17351,7 +17369,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="220" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D32" s="220" t="str">
         <f aca="false" t="array" ref="D32:D32">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17361,13 +17379,13 @@
         <v>45778</v>
       </c>
       <c r="G32" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H32" s="220" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="I32" s="220" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="J32" s="387" t="n">
         <v>192168203223</v>
@@ -17403,13 +17421,13 @@
         <v>45778</v>
       </c>
       <c r="G33" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H33" s="220" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="I33" s="220" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="J33" s="387" t="n">
         <v>192168203255</v>
@@ -17435,26 +17453,26 @@
         <v>3</v>
       </c>
       <c r="C34" s="388" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D34" s="388" t="str">
         <f aca="false" t="array" ref="D34:D34">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E34" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G34" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H34" s="220" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I34" s="220" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="J34" s="220" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="K34" s="220" t="n">
         <v>1033</v>
@@ -17477,7 +17495,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="220" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="D35" s="220" t="str">
         <f aca="false" t="array" ref="D35:D35">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17487,16 +17505,16 @@
         <v>45770</v>
       </c>
       <c r="G35" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H35" s="220" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="I35" s="220" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="J35" s="220" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="K35" s="220" t="n">
         <v>1034</v>
@@ -17519,26 +17537,26 @@
         <v>3</v>
       </c>
       <c r="C36" s="220" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="D36" s="220" t="str">
         <f aca="false" t="array" ref="D36:D36">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E36" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G36" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H36" s="220" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="I36" s="220" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="J36" s="220" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="K36" s="220" t="n">
         <v>1035</v>
@@ -17561,7 +17579,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="220" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="D37" s="220" t="str">
         <f aca="false" t="array" ref="D37:D37">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17571,13 +17589,13 @@
         <v>45771</v>
       </c>
       <c r="G37" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H37" s="220" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="I37" s="220" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="J37" s="387" t="n">
         <v>192168204127</v>
@@ -17603,7 +17621,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="220" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D38" s="220" t="str">
         <f aca="false" t="array" ref="D38:D38">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17613,13 +17631,13 @@
         <v>45771</v>
       </c>
       <c r="G38" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H38" s="220" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="I38" s="220" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="J38" s="387" t="n">
         <v>192168204159</v>
@@ -17645,7 +17663,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="220" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D39" s="220" t="str">
         <f aca="false" t="array" ref="D39:D39">_xlfn.XLOOKUP(Tabla4[ROOM],Tabla14[Villa],Tabla14['# Serie],"No se Encontro",0,1)</f>
@@ -17655,13 +17673,13 @@
         <v>45774</v>
       </c>
       <c r="G39" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H39" s="220" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="I39" s="220" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="J39" s="387" t="n">
         <v>192168204191</v>
@@ -17697,13 +17715,13 @@
         <v>45771</v>
       </c>
       <c r="G40" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H40" s="220" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="I40" s="220" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="J40" s="387" t="n">
         <v>192168204223</v>
@@ -17736,16 +17754,16 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E41" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G41" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H41" s="220" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="I41" s="220" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="J41" s="387" t="n">
         <v>192168204255</v>
@@ -17778,19 +17796,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E42" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G42" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H42" s="220" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="I42" s="220" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="J42" s="220" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="K42" s="220" t="n">
         <v>1041</v>
@@ -17823,16 +17841,16 @@
         <v>45771</v>
       </c>
       <c r="G43" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H43" s="220" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="I43" s="220" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="J43" s="220" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="K43" s="220" t="n">
         <v>1042</v>
@@ -17865,16 +17883,16 @@
         <v>45771</v>
       </c>
       <c r="G44" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H44" s="220" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="I44" s="220" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="J44" s="220" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="K44" s="220" t="n">
         <v>1043</v>
@@ -17907,13 +17925,13 @@
         <v>45771</v>
       </c>
       <c r="G45" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H45" s="220" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="I45" s="220" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="J45" s="387" t="n">
         <v>192168205127</v>
@@ -17949,13 +17967,13 @@
         <v>45772</v>
       </c>
       <c r="G46" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H46" s="220" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="I46" s="220" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="J46" s="387" t="n">
         <v>192168205159</v>
@@ -17991,13 +18009,13 @@
         <v>45774</v>
       </c>
       <c r="G47" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H47" s="220" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="I47" s="220" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="J47" s="387" t="n">
         <v>192168205191</v>
@@ -18033,13 +18051,13 @@
         <v>45774</v>
       </c>
       <c r="G48" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H48" s="220" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="I48" s="220" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="J48" s="387" t="n">
         <v>192168205223</v>
@@ -18075,13 +18093,13 @@
         <v>45773</v>
       </c>
       <c r="G49" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H49" s="220" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="I49" s="220" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="J49" s="387" t="n">
         <v>192168205255</v>
@@ -18117,16 +18135,16 @@
         <v>45772</v>
       </c>
       <c r="G50" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H50" s="220" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="I50" s="220" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="J50" s="220" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="K50" s="220" t="n">
         <v>1049</v>
@@ -18156,19 +18174,19 @@
         <v>CNQ4KPPRY4</v>
       </c>
       <c r="E51" s="382" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G51" s="221" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H51" s="220" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="I51" s="220" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="J51" s="220" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="K51" s="220" t="n">
         <v>1050</v>
@@ -18184,7 +18202,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="381" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B52" s="220" t="str">
         <f aca="false">LEFT(A52)</f>
@@ -18198,13 +18216,13 @@
       <c r="F52" s="382"/>
       <c r="G52" s="221"/>
       <c r="H52" s="220" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="I52" s="220" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="J52" s="220" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="K52" s="220" t="n">
         <v>1051</v>
@@ -18213,7 +18231,7 @@
         <v>123456789</v>
       </c>
       <c r="O52" s="220" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21325,10 +21343,10 @@
         <v>512</v>
       </c>
       <c r="B1" s="390" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="C1" s="390" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="D1" s="362"/>
     </row>
@@ -21358,7 +21376,7 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="395" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="B4" s="396" t="n">
         <v>45770</v>
@@ -21370,7 +21388,7 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="391" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B5" s="392" t="n">
         <v>45773</v>

</xml_diff>